<commit_message>
1des fpoo aula05 correcao
</commit_message>
<xml_diff>
--- a/1des/chamada.xlsx
+++ b/1des/chamada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\senai2022\1des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A878CF19-8D03-4985-9C36-90991B33F6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB8C1CD-BCD5-420B-AEBD-2D760C3EEB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16894AAC-534F-4800-A9CE-F9EFF9F0773F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{16894AAC-534F-4800-A9CE-F9EFF9F0773F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="58">
   <si>
     <t>Ana Maria Duarte Campelo</t>
   </si>
@@ -583,7 +583,10 @@
   <dimension ref="A1:Y51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,6 +814,9 @@
       <c r="U3" t="s">
         <v>55</v>
       </c>
+      <c r="V3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -876,6 +882,9 @@
       <c r="U4" t="s">
         <v>55</v>
       </c>
+      <c r="V4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -941,6 +950,9 @@
       <c r="U5" t="s">
         <v>55</v>
       </c>
+      <c r="V5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1006,6 +1018,9 @@
       <c r="U6" t="s">
         <v>55</v>
       </c>
+      <c r="V6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1071,6 +1086,9 @@
       <c r="U7" t="s">
         <v>55</v>
       </c>
+      <c r="V7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1136,6 +1154,9 @@
       <c r="U8" t="s">
         <v>56</v>
       </c>
+      <c r="V8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1201,6 +1222,9 @@
       <c r="U9" t="s">
         <v>55</v>
       </c>
+      <c r="V9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1266,6 +1290,9 @@
       <c r="U10" t="s">
         <v>55</v>
       </c>
+      <c r="V10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1331,6 +1358,9 @@
       <c r="U11" t="s">
         <v>55</v>
       </c>
+      <c r="V11" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1396,6 +1426,9 @@
       <c r="U12" t="s">
         <v>56</v>
       </c>
+      <c r="V12" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1461,6 +1494,9 @@
       <c r="U13" t="s">
         <v>55</v>
       </c>
+      <c r="V13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1526,6 +1562,9 @@
       <c r="U14" t="s">
         <v>55</v>
       </c>
+      <c r="V14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1591,6 +1630,9 @@
       <c r="U15" t="s">
         <v>55</v>
       </c>
+      <c r="V15" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1656,8 +1698,11 @@
       <c r="U16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1721,8 +1766,11 @@
       <c r="U17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
@@ -1786,8 +1834,11 @@
       <c r="U18" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V18" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
@@ -1851,8 +1902,11 @@
       <c r="U19" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V19" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1916,8 +1970,11 @@
       <c r="U20" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1981,8 +2038,11 @@
       <c r="U21" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2046,8 +2106,11 @@
       <c r="U22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2111,8 +2174,11 @@
       <c r="U23" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2176,8 +2242,11 @@
       <c r="U24" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -2241,8 +2310,11 @@
       <c r="U25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2306,8 +2378,11 @@
       <c r="U26" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2371,8 +2446,11 @@
       <c r="U27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -2436,8 +2514,11 @@
       <c r="U28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>31</v>
       </c>
@@ -2501,8 +2582,11 @@
       <c r="U29" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V29" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>52</v>
       </c>
@@ -2566,8 +2650,11 @@
       <c r="U30" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V30" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2631,8 +2718,11 @@
       <c r="U31" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -2696,8 +2786,11 @@
       <c r="U32" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2761,8 +2854,11 @@
       <c r="U33" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>53</v>
       </c>
@@ -2826,8 +2922,11 @@
       <c r="U34" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V34" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -2891,8 +2990,11 @@
       <c r="U35" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -2956,8 +3058,11 @@
       <c r="U36" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -3021,8 +3126,11 @@
       <c r="U37" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -3086,8 +3194,11 @@
       <c r="U38" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>16</v>
       </c>
@@ -3151,8 +3262,11 @@
       <c r="U39" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V39" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -3216,8 +3330,11 @@
       <c r="U40" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>54</v>
       </c>
@@ -3281,8 +3398,11 @@
       <c r="U41" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V41" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -3346,8 +3466,11 @@
       <c r="U42" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -3399,8 +3522,11 @@
       <c r="U43" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -3452,8 +3578,11 @@
       <c r="U44" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -3472,8 +3601,11 @@
       <c r="U45" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -3492,8 +3624,11 @@
       <c r="U46" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>38</v>
       </c>
@@ -3524,8 +3659,11 @@
       <c r="U47" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V47" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -3568,8 +3706,11 @@
       <c r="U48" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -3612,8 +3753,11 @@
       <c r="U49" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -3650,8 +3794,11 @@
       <c r="U50" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -3662,6 +3809,9 @@
         <v>55</v>
       </c>
       <c r="U51" t="s">
+        <v>55</v>
+      </c>
+      <c r="V51" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1des fpoo aula17 e 18
</commit_message>
<xml_diff>
--- a/1des/chamada.xlsx
+++ b/1des/chamada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\senai2022\1des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C54A71-3E35-46F5-86A6-DC51EC126B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF289E7-FE2F-48E3-8A86-5C93B1CEEE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{16894AAC-534F-4800-A9CE-F9EFF9F0773F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16894AAC-534F-4800-A9CE-F9EFF9F0773F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3691" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3726" uniqueCount="60">
   <si>
     <t>Ana Maria Duarte Campelo</t>
   </si>
@@ -639,11 +639,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CF2F16-AB51-4356-B13B-717A13C6773A}">
   <dimension ref="A1:DJ51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="BT6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="BT3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="CM49" sqref="CM49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,6 +1457,9 @@
       <c r="CL3" t="s">
         <v>56</v>
       </c>
+      <c r="CM3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:95" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1729,6 +1732,9 @@
       <c r="CL4" t="s">
         <v>56</v>
       </c>
+      <c r="CM4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2001,6 +2007,9 @@
       <c r="CL5" t="s">
         <v>55</v>
       </c>
+      <c r="CM5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2273,6 +2282,9 @@
       <c r="CL6" t="s">
         <v>55</v>
       </c>
+      <c r="CM6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2545,6 +2557,9 @@
       <c r="CL7" t="s">
         <v>55</v>
       </c>
+      <c r="CM7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2817,6 +2832,9 @@
       <c r="CL8" t="s">
         <v>56</v>
       </c>
+      <c r="CM8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="9" spans="1:95" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -3402,6 +3420,9 @@
       <c r="CL12" t="s">
         <v>55</v>
       </c>
+      <c r="CM12" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3674,6 +3695,9 @@
       <c r="CL13" t="s">
         <v>55</v>
       </c>
+      <c r="CM13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3946,6 +3970,9 @@
       <c r="CL14" t="s">
         <v>56</v>
       </c>
+      <c r="CM14" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="1:95" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -4465,6 +4492,9 @@
       <c r="CL17" t="s">
         <v>55</v>
       </c>
+      <c r="CM17" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="18" spans="1:114" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -4737,7 +4767,9 @@
       <c r="CL18" t="s">
         <v>55</v>
       </c>
-      <c r="CM18"/>
+      <c r="CM18" t="s">
+        <v>55</v>
+      </c>
       <c r="CN18"/>
       <c r="CO18"/>
       <c r="CP18"/>
@@ -5025,7 +5057,9 @@
       <c r="CL19" t="s">
         <v>55</v>
       </c>
-      <c r="CM19"/>
+      <c r="CM19" t="s">
+        <v>55</v>
+      </c>
       <c r="CN19"/>
       <c r="CO19"/>
       <c r="CP19"/>
@@ -5321,6 +5355,9 @@
       <c r="CL20" t="s">
         <v>55</v>
       </c>
+      <c r="CM20" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -5593,6 +5630,9 @@
       <c r="CL21" t="s">
         <v>55</v>
       </c>
+      <c r="CM21" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="22" spans="1:114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -5974,6 +6014,9 @@
       <c r="CL23" t="s">
         <v>55</v>
       </c>
+      <c r="CM23" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="24" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -6195,6 +6238,9 @@
       <c r="CL24" t="s">
         <v>56</v>
       </c>
+      <c r="CM24" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -6467,6 +6513,9 @@
       <c r="CL25" t="s">
         <v>55</v>
       </c>
+      <c r="CM25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="26" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -6739,6 +6788,9 @@
       <c r="CL26" t="s">
         <v>55</v>
       </c>
+      <c r="CM26" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="27" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -7011,6 +7063,9 @@
       <c r="CL27" t="s">
         <v>55</v>
       </c>
+      <c r="CM27" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="1:114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -7390,7 +7445,9 @@
       <c r="CL29" t="s">
         <v>55</v>
       </c>
-      <c r="CM29"/>
+      <c r="CM29" t="s">
+        <v>55</v>
+      </c>
       <c r="CN29"/>
       <c r="CO29"/>
       <c r="CP29"/>
@@ -7686,7 +7743,9 @@
       <c r="CL30" t="s">
         <v>55</v>
       </c>
-      <c r="CM30"/>
+      <c r="CM30" t="s">
+        <v>55</v>
+      </c>
       <c r="CN30"/>
       <c r="CO30"/>
       <c r="CP30"/>
@@ -8091,6 +8150,9 @@
       <c r="CL32" t="s">
         <v>56</v>
       </c>
+      <c r="CM32" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="33" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -8362,6 +8424,9 @@
       </c>
       <c r="CL33" t="s">
         <v>56</v>
+      </c>
+      <c r="CM33" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:114" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -9019,6 +9084,9 @@
       <c r="CL36" t="s">
         <v>55</v>
       </c>
+      <c r="CM36" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="37" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -9291,6 +9359,9 @@
       <c r="CL37" t="s">
         <v>56</v>
       </c>
+      <c r="CM37" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="38" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -9561,6 +9632,9 @@
         <v>55</v>
       </c>
       <c r="CL38" t="s">
+        <v>55</v>
+      </c>
+      <c r="CM38" t="s">
         <v>55</v>
       </c>
     </row>
@@ -9983,6 +10057,9 @@
       <c r="CL40" t="s">
         <v>55</v>
       </c>
+      <c r="CM40" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="41" spans="1:114" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -10518,6 +10595,9 @@
       <c r="CL43" t="s">
         <v>56</v>
       </c>
+      <c r="CM43" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="44" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -10790,6 +10870,9 @@
       <c r="CL44" t="s">
         <v>56</v>
       </c>
+      <c r="CM44" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="45" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -11062,6 +11145,9 @@
       <c r="CL45" t="s">
         <v>55</v>
       </c>
+      <c r="CM45" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="46" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -11288,6 +11374,9 @@
       </c>
       <c r="CL46" t="s">
         <v>55</v>
+      </c>
+      <c r="CM46" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:114" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -11547,7 +11636,9 @@
       <c r="CL47" t="s">
         <v>55</v>
       </c>
-      <c r="CM47"/>
+      <c r="CM47" t="s">
+        <v>55</v>
+      </c>
       <c r="CN47"/>
       <c r="CO47"/>
       <c r="CP47"/>
@@ -11712,7 +11803,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -11983,8 +12074,11 @@
       <c r="CL49" t="s">
         <v>55</v>
       </c>
+      <c r="CM49" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="50" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -12234,8 +12328,11 @@
       <c r="CL50" t="s">
         <v>55</v>
       </c>
+      <c r="CM50" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="51" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -12504,6 +12601,9 @@
         <v>55</v>
       </c>
       <c r="CL51" t="s">
+        <v>55</v>
+      </c>
+      <c r="CM51" t="s">
         <v>55</v>
       </c>
     </row>
@@ -12531,7 +12631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643C73D0-CDBB-4A7D-912C-7FC0A3BE6CDB}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1des fpoo java GUI
</commit_message>
<xml_diff>
--- a/1des/chamada.xlsx
+++ b/1des/chamada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\senai2022\1des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75E3B57-FDE2-46B7-82B4-D6520B0D33DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73190071-BC5D-4241-A1EC-905B4B138FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{16894AAC-534F-4800-A9CE-F9EFF9F0773F}"/>
+    <workbookView xWindow="1365" yWindow="45" windowWidth="27165" windowHeight="15315" xr2:uid="{16894AAC-534F-4800-A9CE-F9EFF9F0773F}"/>
   </bookViews>
   <sheets>
     <sheet name="Chamada" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4159" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4199" uniqueCount="62">
   <si>
     <t>Ana Maria Duarte Campelo</t>
   </si>
@@ -734,10 +734,10 @@
   <dimension ref="A1:DJ51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="BT3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="CB3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CU51" sqref="CU51"/>
+      <selection pane="bottomRight" activeCell="CW46" sqref="CW46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,10 +751,10 @@
     <col min="41" max="55" width="6.5703125" customWidth="1"/>
     <col min="56" max="76" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="77" max="98" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="99" max="100" width="7" bestFit="1" customWidth="1"/>
+    <col min="99" max="105" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>40</v>
       </c>
@@ -1053,8 +1053,23 @@
       <c r="CV1" s="2">
         <v>44897</v>
       </c>
-    </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CW1" s="2">
+        <v>44900</v>
+      </c>
+      <c r="CX1" s="2">
+        <v>44901</v>
+      </c>
+      <c r="CY1" s="2">
+        <v>44902</v>
+      </c>
+      <c r="CZ1" s="2">
+        <v>44903</v>
+      </c>
+      <c r="DA1" s="2">
+        <v>44904</v>
+      </c>
+    </row>
+    <row r="2" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
@@ -1355,8 +1370,23 @@
       <c r="CV2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CW2" t="s">
+        <v>43</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>44</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>41</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>42</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:105" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1612,8 +1642,11 @@
       <c r="CV3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:100" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CW3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:105" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1914,8 +1947,11 @@
       <c r="CV4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CW4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2216,8 +2252,11 @@
       <c r="CV5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CW5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2518,8 +2557,11 @@
       <c r="CV6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CW6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2820,8 +2862,11 @@
       <c r="CV7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CW7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3122,8 +3167,11 @@
       <c r="CV8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:100" hidden="1" x14ac:dyDescent="0.25">
+      <c r="CW8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>51</v>
       </c>
@@ -3232,7 +3280,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:100" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -3327,7 +3375,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:100" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>52</v>
       </c>
@@ -3436,7 +3484,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -3737,8 +3785,11 @@
       <c r="CV12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CW12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -4039,8 +4090,11 @@
       <c r="CV13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CW13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
@@ -4341,8 +4395,11 @@
       <c r="CV14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:100" hidden="1" x14ac:dyDescent="0.25">
+      <c r="CW14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -4464,7 +4521,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:100" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4890,6 +4947,9 @@
       <c r="CV17" t="s">
         <v>55</v>
       </c>
+      <c r="CW17" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="18" spans="1:114" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -5192,7 +5252,9 @@
       <c r="CV18" t="s">
         <v>55</v>
       </c>
-      <c r="CW18"/>
+      <c r="CW18" t="s">
+        <v>55</v>
+      </c>
       <c r="CX18"/>
       <c r="CY18"/>
       <c r="CZ18"/>
@@ -5500,7 +5562,9 @@
       <c r="CV19" t="s">
         <v>55</v>
       </c>
-      <c r="CW19"/>
+      <c r="CW19" t="s">
+        <v>55</v>
+      </c>
       <c r="CX19"/>
       <c r="CY19"/>
       <c r="CZ19"/>
@@ -5816,6 +5880,9 @@
       <c r="CV20" t="s">
         <v>55</v>
       </c>
+      <c r="CW20" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -6118,6 +6185,9 @@
       <c r="CV21" t="s">
         <v>55</v>
       </c>
+      <c r="CW21" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="22" spans="1:114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -6529,6 +6599,9 @@
       <c r="CV23" t="s">
         <v>55</v>
       </c>
+      <c r="CW23" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="24" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -6780,6 +6853,9 @@
       <c r="CV24" t="s">
         <v>56</v>
       </c>
+      <c r="CW24" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -7082,6 +7158,9 @@
       <c r="CV25" t="s">
         <v>55</v>
       </c>
+      <c r="CW25" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -7384,6 +7463,9 @@
       <c r="CV26" t="s">
         <v>55</v>
       </c>
+      <c r="CW26" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="27" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -7686,6 +7768,9 @@
       <c r="CV27" t="s">
         <v>55</v>
       </c>
+      <c r="CW27" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="1:114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -8095,7 +8180,9 @@
       <c r="CV29" t="s">
         <v>55</v>
       </c>
-      <c r="CW29"/>
+      <c r="CW29" t="s">
+        <v>55</v>
+      </c>
       <c r="CX29"/>
       <c r="CY29"/>
       <c r="CZ29"/>
@@ -8411,7 +8498,9 @@
       <c r="CV30" t="s">
         <v>55</v>
       </c>
-      <c r="CW30"/>
+      <c r="CW30" t="s">
+        <v>55</v>
+      </c>
       <c r="CX30"/>
       <c r="CY30"/>
       <c r="CZ30"/>
@@ -8836,6 +8925,9 @@
       <c r="CV32" t="s">
         <v>55</v>
       </c>
+      <c r="CW32" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="33" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -9136,6 +9228,9 @@
         <v>55</v>
       </c>
       <c r="CV33" t="s">
+        <v>55</v>
+      </c>
+      <c r="CW33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -9824,6 +9919,9 @@
       <c r="CV36" t="s">
         <v>55</v>
       </c>
+      <c r="CW36" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="37" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -10126,6 +10224,9 @@
       <c r="CV37" t="s">
         <v>56</v>
       </c>
+      <c r="CW37" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="38" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -10426,6 +10527,9 @@
         <v>55</v>
       </c>
       <c r="CV38" t="s">
+        <v>55</v>
+      </c>
+      <c r="CW38" t="s">
         <v>55</v>
       </c>
     </row>
@@ -10878,6 +10982,9 @@
       <c r="CV40" t="s">
         <v>55</v>
       </c>
+      <c r="CW40" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="41" spans="1:114" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -11443,6 +11550,9 @@
       <c r="CV43" t="s">
         <v>56</v>
       </c>
+      <c r="CW43" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="44" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -11745,6 +11855,9 @@
       <c r="CV44" t="s">
         <v>55</v>
       </c>
+      <c r="CW44" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="45" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -12047,6 +12160,9 @@
       <c r="CV45" t="s">
         <v>55</v>
       </c>
+      <c r="CW45" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="46" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -12302,6 +12418,9 @@
         <v>55</v>
       </c>
       <c r="CV46" t="s">
+        <v>55</v>
+      </c>
+      <c r="CW46" t="s">
         <v>55</v>
       </c>
     </row>
@@ -12592,7 +12711,9 @@
       <c r="CV47" t="s">
         <v>55</v>
       </c>
-      <c r="CW47"/>
+      <c r="CW47" t="s">
+        <v>55</v>
+      </c>
       <c r="CX47"/>
       <c r="CY47"/>
       <c r="CZ47"/>
@@ -12747,7 +12868,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -13048,8 +13169,11 @@
       <c r="CV49" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="50" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CW49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -13329,8 +13453,11 @@
       <c r="CV50" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="51" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="CW50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -13629,6 +13756,9 @@
         <v>55</v>
       </c>
       <c r="CV51" t="s">
+        <v>55</v>
+      </c>
+      <c r="CW51" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>